<commit_message>
Renaming the drifters and ctd data files for 2022 data
</commit_message>
<xml_diff>
--- a/Data/2022/Day1/logsheet.xlsx
+++ b/Data/2022/Day1/logsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olanr\Downloads\MIRDriftersAndCTDs\OtherDaysData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olanr\Downloads\OceanographyAnalysis\Data\2022\Day1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8969B80F-AAD0-4E58-88DE-CBBB05438E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78ED6E32-1A55-4B06-AD87-0B78330D785D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14505" yWindow="2820" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>Station</t>
   </si>
@@ -120,24 +120,15 @@
     <t>-</t>
   </si>
   <si>
-    <t>CTD-ST1</t>
-  </si>
-  <si>
     <t>6º 0.587'</t>
   </si>
   <si>
-    <t>CTD-ST2</t>
-  </si>
-  <si>
     <t>6º 0.697'</t>
   </si>
   <si>
     <t>43º 4.913'</t>
   </si>
   <si>
-    <t>CTD-ST3</t>
-  </si>
-  <si>
     <t>5º 59.088'</t>
   </si>
   <si>
@@ -154,6 +145,9 @@
   </si>
   <si>
     <t>WD</t>
+  </si>
+  <si>
+    <t>CTD</t>
   </si>
 </sst>
 </file>
@@ -454,7 +448,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -471,7 +465,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -503,7 +497,7 @@
         <v>273</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="4">
         <v>0.43611111111111112</v>
@@ -532,7 +526,7 @@
         <v>9666</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D3" s="4">
         <v>0.43611111111111112</v>
@@ -561,7 +555,7 @@
         <v>6439</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4">
         <v>0.43611111111111112</v>
@@ -590,7 +584,7 @@
         <v>274</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="5">
         <v>0.44583333333333336</v>
@@ -619,7 +613,7 @@
         <v>8436</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="5">
         <v>0.44583333333333336</v>
@@ -648,7 +642,7 @@
         <v>3368</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7" s="5">
         <v>0.44583333333333336</v>
@@ -677,7 +671,7 @@
         <v>7230</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D8" s="4">
         <v>0.46250000000000002</v>
@@ -706,7 +700,7 @@
         <v>119</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9" s="5">
         <v>0.46250000000000002</v>
@@ -735,7 +729,7 @@
         <v>277</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D10" s="5">
         <v>0.46250000000000002</v>
@@ -764,7 +758,7 @@
         <v>2052</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4">
         <v>0.48819444444444443</v>
@@ -789,15 +783,17 @@
       <c r="A12" s="3">
         <v>4</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="3"/>
+      <c r="B12" s="3">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D12" s="4">
         <v>0.49027777777777776</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>29</v>
@@ -806,7 +802,7 @@
         <v>0.50347222222222221</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>29</v>
@@ -816,54 +812,58 @@
       <c r="A13" s="3">
         <v>5</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="3"/>
+      <c r="B13" s="6">
+        <v>2</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D13" s="4">
         <v>0.54652777777777772</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" s="4">
         <v>0.54861111111111116</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>6</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="3"/>
+      <c r="B14" s="6">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="D14" s="4">
         <v>0.55763888888888891</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G14" s="4">
         <v>0.56180555555555556</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>